<commit_message>
Aenderungen zum großen Teil eingebaut
</commit_message>
<xml_diff>
--- a/raw_inputs/economics.xlsx
+++ b/raw_inputs/economics.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Forschung\EBC0324_BMWi_BF2016_tos\Students\tos-sre\03_Optimierungsprogramm\raw_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Subsidy-Optimization\raw_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="103">
   <si>
     <t>Euro / kWh</t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>pel_sta</t>
+  </si>
+  <si>
+    <t>prChange_pellet</t>
+  </si>
+  <si>
+    <t>Price change factors per year for pellets</t>
   </si>
 </sst>
 </file>
@@ -743,15 +749,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -840,58 +847,72 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>101</v>
       </c>
       <c r="B7">
-        <v>1.0251999999999999</v>
+        <v>1.03</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>1.0169999999999999</v>
+        <v>1.0251999999999999</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>96</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <f>0.03284+0.005</f>
         <v>3.7839999999999999E-2</v>
       </c>
-      <c r="C9" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="13" t="s">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>5.4999999999999997E-3</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>35</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>98</v>
       </c>
     </row>
@@ -906,7 +927,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="C25:D27"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -993,7 +1014,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1426,7 +1447,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1470,7 +1491,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Version vor Entfernen der versch. Tarife und überflüssigen Variablen
</commit_message>
<xml_diff>
--- a/raw_inputs/economics.xlsx
+++ b/raw_inputs/economics.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="12855"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="12855" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="gen_economics" sheetId="1" r:id="rId1"/>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,7 +747,7 @@
         <v>16</v>
       </c>
       <c r="B2">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>15</v>
@@ -2667,8 +2667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F9:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,7 +2712,7 @@
         <v>24</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="C3" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
changed some parameters to upper limit
</commit_message>
<xml_diff>
--- a/raw_inputs/economics.xlsx
+++ b/raw_inputs/economics.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Forschung\EBC0324_BMWi_BF2016_tos\Students\srm-jba\Programme\Subsidy-Optimization-Vent\raw_inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Dokumente\GitHub\Subsidy-Optimization\raw_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_31147260F503E99FD7A742065CC714366850218A" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00105C8A-2B14-4A30-8153-E0126E7FDDF4}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="12855" activeTab="7"/>
+    <workbookView xWindow="14385" yWindow="-15" windowWidth="14430" windowHeight="12855" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gen_economics" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,14 @@
     <sheet name="ep_table" sheetId="10" r:id="rId7"/>
     <sheet name="further_parameters" sheetId="2" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -307,7 +315,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -505,6 +513,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -540,6 +565,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -715,20 +757,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -742,7 +784,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -756,7 +798,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -770,7 +812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -784,7 +826,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -798,7 +840,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -812,7 +854,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -826,7 +868,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -840,7 +882,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -854,7 +896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>78</v>
       </c>
@@ -869,7 +911,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -890,23 +932,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" customWidth="1"/>
-    <col min="3" max="3" width="50.85546875" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.86328125" customWidth="1"/>
+    <col min="3" max="3" width="50.86328125" customWidth="1"/>
+    <col min="4" max="4" width="27.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -923,7 +965,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -943,35 +985,38 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{4BE99866-580D-4AF3-A15A-FF18D9969129}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="61.140625" customWidth="1"/>
+    <col min="2" max="2" width="61.1328125" customWidth="1"/>
     <col min="3" max="3" width="65" customWidth="1"/>
-    <col min="6" max="6" width="78.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="78.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -991,7 +1036,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -1014,7 +1059,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>40</v>
       </c>
@@ -1037,7 +1082,7 @@
         <v>42572</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B5" s="3"/>
     </row>
   </sheetData>
@@ -1046,23 +1091,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1328125" customWidth="1"/>
+    <col min="2" max="2" width="50.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -1079,7 +1124,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -1095,7 +1140,7 @@
       <c r="E2" s="2"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="E3" s="2"/>
       <c r="F3" s="1"/>
     </row>
@@ -1105,21 +1150,21 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1130,7 +1175,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1141,7 +1186,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1152,7 +1197,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1163,7 +1208,7 @@
         <v>21500</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -1174,7 +1219,7 @@
         <v>8800</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -1185,7 +1230,7 @@
         <v>5300</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -1196,7 +1241,7 @@
         <v>3100</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -1207,7 +1252,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -1218,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1229,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -1246,22 +1291,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.86328125" customWidth="1"/>
+    <col min="2" max="2" width="9.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1278,7 +1323,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1295,7 +1340,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>65</v>
       </c>
@@ -1312,7 +1357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>66</v>
       </c>
@@ -1329,7 +1374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1346,17 +1391,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>73</v>
       </c>
@@ -1367,22 +1412,22 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="10" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="10" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="7"/>
       <c r="B1" s="8" t="s">
         <v>58</v>
@@ -1415,7 +1460,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1447,7 +1492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="9">
         <v>2</v>
       </c>
@@ -1480,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <v>3</v>
       </c>
@@ -1512,7 +1557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="9">
         <v>4</v>
       </c>
@@ -1545,7 +1590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <v>5</v>
       </c>
@@ -1577,7 +1622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="9">
         <v>6</v>
       </c>
@@ -1610,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="6">
         <v>7</v>
       </c>
@@ -1645,7 +1690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="9">
         <v>8</v>
       </c>
@@ -1680,7 +1725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
         <v>9</v>
       </c>
@@ -1715,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="9">
         <v>10</v>
       </c>
@@ -1750,7 +1795,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <v>11</v>
       </c>
@@ -1785,7 +1830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="9">
         <v>12</v>
       </c>
@@ -1820,7 +1865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1855,7 +1900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="9">
         <v>14</v>
       </c>
@@ -1890,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <v>15</v>
       </c>
@@ -1925,7 +1970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="9">
         <v>16</v>
       </c>
@@ -1960,7 +2005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <v>17</v>
       </c>
@@ -1995,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="9">
         <v>18</v>
       </c>
@@ -2030,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="6">
         <v>19</v>
       </c>
@@ -2065,7 +2110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="9">
         <v>20</v>
       </c>
@@ -2100,7 +2145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <v>21</v>
       </c>
@@ -2135,7 +2180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="9">
         <v>22</v>
       </c>
@@ -2170,7 +2215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -2205,7 +2250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="9">
         <v>24</v>
       </c>
@@ -2240,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -2275,7 +2320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="9">
         <v>26</v>
       </c>
@@ -2310,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <v>27</v>
       </c>
@@ -2345,7 +2390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="9">
         <v>28</v>
       </c>
@@ -2380,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="6">
         <v>29</v>
       </c>
@@ -2415,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="9">
         <v>30</v>
       </c>
@@ -2450,7 +2495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
@@ -2459,7 +2504,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
@@ -2468,7 +2513,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
@@ -2477,7 +2522,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
@@ -2486,7 +2531,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
@@ -2495,7 +2540,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
@@ -2504,7 +2549,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
@@ -2513,7 +2558,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D39" s="5"/>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -2522,7 +2567,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -2531,7 +2576,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -2540,7 +2585,7 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -2549,7 +2594,7 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -2558,7 +2603,7 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -2567,7 +2612,7 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D45" s="5"/>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2576,7 +2621,7 @@
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D46" s="5"/>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -2585,7 +2630,7 @@
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -2594,7 +2639,7 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -2603,7 +2648,7 @@
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
-    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D49" s="5"/>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -2612,7 +2657,7 @@
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D50" s="5"/>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
@@ -2621,7 +2666,7 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D51" s="5"/>
       <c r="E51" s="5"/>
       <c r="F51" s="5"/>
@@ -2630,7 +2675,7 @@
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
-    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D52" s="5"/>
       <c r="E52" s="5"/>
       <c r="F52" s="5"/>
@@ -2639,7 +2684,7 @@
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
-    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
       <c r="F53" s="5"/>
@@ -2648,7 +2693,7 @@
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:10" x14ac:dyDescent="0.45">
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
@@ -2664,22 +2709,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -2693,7 +2738,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2707,7 +2752,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -2721,7 +2766,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -2735,7 +2780,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>28</v>
       </c>

</xml_diff>